<commit_message>
modifications in gitignore, readme and in the data
</commit_message>
<xml_diff>
--- a/data/raw_data/spending.xlsx
+++ b/data/raw_data/spending.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petiakovacs/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petiakovacs/Documents/travel_expenses/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC201FE-506E-B146-9A48-846C64CAF650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B029724-2A3D-5841-B389-2B7624C1E6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2843,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="I419" sqref="I419"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>